<commit_message>
Alterado excel para código inep
</commit_message>
<xml_diff>
--- a/WebContent/ListaAlunos.xlsx
+++ b/WebContent/ListaAlunos.xlsx
@@ -24,9 +24,6 @@
     <t>PROFESSOR</t>
   </si>
   <si>
-    <t>ESCOLA</t>
-  </si>
-  <si>
     <t>NOME COMPLETO DO ALUNO</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>Menino</t>
+  </si>
+  <si>
+    <t>CODIGO INEP DA ESCOLA</t>
   </si>
 </sst>
 </file>
@@ -524,41 +524,41 @@
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="5"/>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="6"/>
       <c r="I2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">

</xml_diff>